<commit_message>
Filtros completos con muestra de filtros activos sin entrar al boton
</commit_message>
<xml_diff>
--- a/Planificación_ISO.xlsx
+++ b/Planificación_ISO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceu365-my.sharepoint.com/personal/victor_vegamartinez_usp_ceu_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorvegamartinez/NasPrivateVictor/uni/2025_2026/ISO/proyectoWeb/Proyecto_Ingenieria_Software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B09ADF-7CC1-4271-91E3-3D7A80053D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15304D20-02D2-E243-9D98-4BA876FAB132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="620" windowWidth="24480" windowHeight="15740" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="620" windowWidth="24480" windowHeight="15760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="260">
   <si>
     <t>Tarea</t>
   </si>
@@ -900,9 +900,6 @@
 </t>
   </si>
   <si>
-    <t>Filtrar por ingredientes, país, usuario, valoracion, dificultad, tiempo y turno de comida en el apartado mis recetas</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Si un usuario accede al apartado Mis recetas tendrá una opción para poder filtrar
 2. Si un usuario selecciona la opción de filtrar deberá aparecer un menú que muestre los diferentes filtros
 3. Al seleccionar un filtro en específico si ese campo son valores libres (no tiene formato predefinido) se mostrará una barra de texto donde podrá introducir los valores a filtrar
@@ -947,12 +944,18 @@
   <si>
     <t>Si el usuario selecciona país de origen al crear/editar una receta le debe aparecer un desplegable con todos los países</t>
   </si>
+  <si>
+    <t>En progreso</t>
+  </si>
+  <si>
+    <t>Filtrar por ingredientes, país, dificultad, tiempo y turno de comida en el apartado mis recetas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,13 +998,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1235,21 +1237,424 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="60">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C5700"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7E6E6"/>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1265,6 +1670,21 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1434,434 +1854,6 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE7E6E6"/>
-          <bgColor rgb="FFE7E6E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC9DAF8"/>
-          <bgColor rgb="FFC9DAF8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1876,7 +1868,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TablaBacklog" displayName="TablaBacklog" ref="A1:H77" headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TablaBacklog" displayName="TablaBacklog" ref="A1:H77" headerRowDxfId="59" dataDxfId="58" totalsRowDxfId="57">
   <autoFilter ref="A1:H77" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
     <filterColumn colId="6">
       <filters>
@@ -1885,14 +1877,14 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{702BA59E-E87C-AF43-BC72-116919A29E64}" name="Criterio de validacion" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6924BD28-A9A8-B84F-AE98-42459B25AAE0}" name="ID" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priority" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tiempo planning poker (horas)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Entrega" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{2C9703D9-E678-1342-81C4-A1629A8FA8A2}" name="Estado" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{702BA59E-E87C-AF43-BC72-116919A29E64}" name="Criterio de validacion" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{6924BD28-A9A8-B84F-AE98-42459B25AAE0}" name="ID" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priority" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tiempo planning poker (horas)" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Entrega" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{2C9703D9-E678-1342-81C4-A1629A8FA8A2}" name="Estado" dataDxfId="49" totalsRowDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2186,20 +2178,20 @@
   <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView topLeftCell="A108" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="36" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001">
+    <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2219,7 +2211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="39.950000000000003">
+    <row r="2" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2240,7 +2232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001">
+    <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -2261,7 +2253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001">
+    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2282,7 +2274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001">
+    <row r="5" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2303,7 +2295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="39.950000000000003">
+    <row r="6" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -2324,7 +2316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="39.950000000000003">
+    <row r="7" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -2345,7 +2337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001">
+    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2366,7 +2358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001">
+    <row r="9" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2387,7 +2379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001">
+    <row r="10" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -2408,7 +2400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39.950000000000003">
+    <row r="11" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -2429,7 +2421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001">
+    <row r="12" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2450,7 +2442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39.950000000000003">
+    <row r="13" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -2471,7 +2463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="39.950000000000003">
+    <row r="14" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -2492,7 +2484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="39.950000000000003">
+    <row r="15" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2513,7 +2505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="39.950000000000003">
+    <row r="16" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -2534,7 +2526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39.950000000000003">
+    <row r="17" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -2555,7 +2547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.100000000000001">
+    <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -2576,7 +2568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001">
+    <row r="19" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -2597,7 +2589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="20.100000000000001">
+    <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -2618,7 +2610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="39.950000000000003">
+    <row r="21" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -2639,7 +2631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="39.950000000000003">
+    <row r="22" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -2660,7 +2652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="20.100000000000001">
+    <row r="23" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
@@ -2681,7 +2673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="20.100000000000001">
+    <row r="24" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -2702,7 +2694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="39.950000000000003">
+    <row r="25" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -2723,7 +2715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="20.100000000000001">
+    <row r="26" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -2741,7 +2733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="39.950000000000003">
+    <row r="27" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
@@ -2762,7 +2754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="39.950000000000003">
+    <row r="28" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
@@ -2783,7 +2775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="20.100000000000001">
+    <row r="29" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
@@ -2804,7 +2796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="39.950000000000003">
+    <row r="30" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -2825,7 +2817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="39.950000000000003">
+    <row r="31" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -2846,7 +2838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>45</v>
       </c>
@@ -2867,7 +2859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="20.100000000000001">
+    <row r="33" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -2888,7 +2880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="39.950000000000003">
+    <row r="34" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
@@ -2909,7 +2901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="39.950000000000003">
+    <row r="35" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
@@ -2930,7 +2922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="39.950000000000003">
+    <row r="36" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>49</v>
       </c>
@@ -2951,7 +2943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="39.950000000000003">
+    <row r="37" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2972,7 +2964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="20.100000000000001">
+    <row r="38" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
@@ -2993,7 +2985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="20.100000000000001">
+    <row r="39" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>53</v>
       </c>
@@ -3014,7 +3006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="39.950000000000003">
+    <row r="40" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
@@ -3035,7 +3027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="39.950000000000003">
+    <row r="41" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -3056,7 +3048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="39.950000000000003">
+    <row r="42" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -3077,7 +3069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="20.100000000000001">
+    <row r="43" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>56</v>
       </c>
@@ -3098,7 +3090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="20.100000000000001">
+    <row r="44" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
@@ -3119,7 +3111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="39.950000000000003">
+    <row r="45" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
@@ -3140,7 +3132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="39.950000000000003">
+    <row r="46" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>59</v>
       </c>
@@ -3161,7 +3153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="39.950000000000003">
+    <row r="47" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>60</v>
       </c>
@@ -3182,7 +3174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="39.950000000000003">
+    <row r="48" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>61</v>
       </c>
@@ -3198,7 +3190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="20.100000000000001">
+    <row r="49" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>62</v>
       </c>
@@ -3219,7 +3211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="39.950000000000003">
+    <row r="50" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>63</v>
       </c>
@@ -3240,7 +3232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="60">
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>64</v>
       </c>
@@ -3261,7 +3253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="39.950000000000003">
+    <row r="52" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>65</v>
       </c>
@@ -3282,7 +3274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="39.950000000000003">
+    <row r="53" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
@@ -3303,7 +3295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="57">
+    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>67</v>
       </c>
@@ -3323,7 +3315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="57">
+    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -3343,7 +3335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="57">
+    <row r="56" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>69</v>
       </c>
@@ -3363,7 +3355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="37.5">
+    <row r="57" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
@@ -3383,7 +3375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="57">
+    <row r="58" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>71</v>
       </c>
@@ -3403,7 +3395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="57">
+    <row r="59" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -3423,7 +3415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="37.5">
+    <row r="60" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
@@ -3444,7 +3436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="57">
+    <row r="61" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>75</v>
       </c>
@@ -3465,7 +3457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="37.5">
+    <row r="62" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>76</v>
       </c>
@@ -3486,7 +3478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="37.5">
+    <row r="63" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>77</v>
       </c>
@@ -3507,7 +3499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="37.5">
+    <row r="64" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>78</v>
       </c>
@@ -3527,7 +3519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="37.5">
+    <row r="65" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>79</v>
       </c>
@@ -3547,7 +3539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="37.5">
+    <row r="66" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>80</v>
       </c>
@@ -3568,7 +3560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="57">
+    <row r="67" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>81</v>
       </c>
@@ -3589,7 +3581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="37.5">
+    <row r="68" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>84</v>
       </c>
@@ -3610,7 +3602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="57">
+    <row r="69" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>85</v>
       </c>
@@ -3631,7 +3623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="37.5">
+    <row r="70" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>87</v>
       </c>
@@ -3649,7 +3641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="37.5">
+    <row r="71" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>88</v>
       </c>
@@ -3667,7 +3659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="37.5">
+    <row r="72" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>90</v>
       </c>
@@ -3685,7 +3677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="37.5">
+    <row r="73" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>91</v>
       </c>
@@ -3703,7 +3695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="18.75">
+    <row r="74" spans="1:15" ht="20" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>94</v>
       </c>
@@ -3725,7 +3717,7 @@
       </c>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="18.75">
+    <row r="75" spans="1:15" ht="20" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>95</v>
       </c>
@@ -3746,7 +3738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="37.5">
+    <row r="76" spans="1:15" ht="40" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>96</v>
       </c>
@@ -3768,7 +3760,7 @@
       </c>
       <c r="M76" s="38"/>
     </row>
-    <row r="77" spans="1:15" ht="37.5">
+    <row r="77" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>97</v>
       </c>
@@ -3789,7 +3781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="57">
+    <row r="78" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>98</v>
       </c>
@@ -3810,7 +3802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="57">
+    <row r="79" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>99</v>
       </c>
@@ -3828,7 +3820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="37.5">
+    <row r="80" spans="1:15" ht="40" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>100</v>
       </c>
@@ -3849,7 +3841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="18.75">
+    <row r="81" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>39</v>
       </c>
@@ -3870,7 +3862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="37.5">
+    <row r="82" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>101</v>
       </c>
@@ -3891,7 +3883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="57">
+    <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>102</v>
       </c>
@@ -3909,7 +3901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="57">
+    <row r="84" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>103</v>
       </c>
@@ -3927,7 +3919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="37.5">
+    <row r="85" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>104</v>
       </c>
@@ -3945,7 +3937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="18.75">
+    <row r="86" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>105</v>
       </c>
@@ -3963,7 +3955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="18.75">
+    <row r="87" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>106</v>
       </c>
@@ -3981,7 +3973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="18.75">
+    <row r="88" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>107</v>
       </c>
@@ -3993,7 +3985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="37.5">
+    <row r="89" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>108</v>
       </c>
@@ -4011,7 +4003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="37.5">
+    <row r="90" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>109</v>
       </c>
@@ -4029,7 +4021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="37.5">
+    <row r="91" spans="1:6" ht="40" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>110</v>
       </c>
@@ -4047,7 +4039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="57">
+    <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>111</v>
       </c>
@@ -4065,7 +4057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="18.75">
+    <row r="93" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>112</v>
       </c>
@@ -4079,13 +4071,13 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="18.75">
+    <row r="94" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D94" s="32"/>
     </row>
-    <row r="95" spans="1:6" ht="18.75">
+    <row r="95" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>115</v>
       </c>
@@ -4103,7 +4095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="57">
+    <row r="96" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
@@ -4121,7 +4113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="35" customFormat="1" ht="56.1" customHeight="1">
+    <row r="97" spans="1:6" s="35" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>118</v>
       </c>
@@ -4142,7 +4134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="35" customFormat="1" ht="75.75">
+    <row r="98" spans="1:6" s="35" customFormat="1" ht="80" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>120</v>
       </c>
@@ -4163,7 +4155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="99" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>121</v>
       </c>
@@ -4184,7 +4176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="35" customFormat="1" ht="57">
+    <row r="100" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>122</v>
       </c>
@@ -4205,7 +4197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="35" customFormat="1" ht="37.35" customHeight="1">
+    <row r="101" spans="1:6" s="35" customFormat="1" ht="37.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>123</v>
       </c>
@@ -4226,7 +4218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="102" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>125</v>
       </c>
@@ -4247,7 +4239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="35" customFormat="1" ht="78.599999999999994" customHeight="1">
+    <row r="103" spans="1:6" s="35" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>126</v>
       </c>
@@ -4268,7 +4260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="104" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>128</v>
       </c>
@@ -4289,7 +4281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="105" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>129</v>
       </c>
@@ -4307,7 +4299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="35" customFormat="1" ht="75.75">
+    <row r="106" spans="1:6" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>130</v>
       </c>
@@ -4317,7 +4309,7 @@
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
     </row>
-    <row r="107" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="107" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>131</v>
       </c>
@@ -4338,7 +4330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="35" customFormat="1" ht="18.75">
+    <row r="108" spans="1:6" s="35" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="36">
         <f>+Requisitos!C59</f>
@@ -4357,7 +4349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="109" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>132</v>
       </c>
@@ -4378,7 +4370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="110" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A110" s="37" t="s">
         <v>133</v>
       </c>
@@ -4399,7 +4391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="35" customFormat="1" ht="18.75">
+    <row r="111" spans="1:6" s="35" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>134</v>
       </c>
@@ -4409,7 +4401,7 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
     </row>
-    <row r="112" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="112" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A112" s="37" t="s">
         <v>135</v>
       </c>
@@ -4419,7 +4411,7 @@
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
     </row>
-    <row r="113" spans="1:6" s="35" customFormat="1" ht="18.75">
+    <row r="113" spans="1:6" s="35" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
@@ -4427,7 +4419,7 @@
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
     </row>
-    <row r="114" spans="1:6" s="35" customFormat="1" ht="37.5">
+    <row r="114" spans="1:6" s="35" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>136</v>
       </c>
@@ -4437,7 +4429,7 @@
       <c r="E114" s="34"/>
       <c r="F114" s="34"/>
     </row>
-    <row r="115" spans="1:6" ht="18.75">
+    <row r="115" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>137</v>
       </c>
@@ -4447,18 +4439,15 @@
       <c r="E115" s="34"/>
       <c r="F115" s="34"/>
     </row>
-    <row r="116" spans="1:6" ht="18.75">
+    <row r="116" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A116" s="35" t="s">
         <v>138</v>
       </c>
       <c r="B116" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E116" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="18.75">
+    </row>
+    <row r="117" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A117" s="35">
         <v>64.650000000000006</v>
       </c>
@@ -4466,7 +4455,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>66.709999999999994</v>
       </c>
@@ -4474,7 +4463,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>140</v>
       </c>
@@ -4484,54 +4473,54 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F32" xr:uid="{74E8B59A-7A92-E349-A281-22786FC7C0A0}"/>
-  <conditionalFormatting sqref="B46:B47 B87 C88:D88 C89:C93 C2:C86">
-    <cfRule type="containsText" dxfId="60" priority="25" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="59" priority="26" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="58" priority="27" operator="containsText" text="Alto"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B107">
-    <cfRule type="containsText" dxfId="57" priority="1" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="56" priority="2" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="55" priority="3" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="46" priority="3" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="Bajo"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109:C109">
-    <cfRule type="containsText" dxfId="54" priority="7" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="53" priority="8" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="Alto"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C86 B46:B47 B87 C88:D88 C89:C93">
+    <cfRule type="containsText" dxfId="41" priority="27" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="39" priority="25" operator="containsText" text="Bajo"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:C97">
-    <cfRule type="containsText" dxfId="51" priority="22" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="50" priority="23" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="49" priority="24" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="38" priority="24" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="37" priority="23" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="36" priority="22" operator="containsText" text="Bajo"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C101">
-    <cfRule type="containsText" dxfId="48" priority="19" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="47" priority="20" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="46" priority="21" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="35" priority="19" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="34" priority="21" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="33" priority="20" operator="containsText" text="Medio"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="45" priority="13" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="44" priority="14" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="43" priority="15" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="32" priority="14" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="31" priority="15" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="30" priority="13" operator="containsText" text="Bajo"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105:C107">
-    <cfRule type="containsText" dxfId="42" priority="10" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="41" priority="11" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="40" priority="12" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="29" priority="12" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="Bajo"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111:C113">
-    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="Bajo"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
       <formula>"En progreso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4551,25 +4540,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="58" style="1" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="71.099999999999994" customHeight="1">
+    <row r="1" spans="1:8" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>141</v>
       </c>
@@ -4595,7 +4584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="279.95" hidden="1">
+    <row r="2" spans="1:8" ht="280" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>148</v>
       </c>
@@ -4621,7 +4610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" hidden="1">
+    <row r="3" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>152</v>
       </c>
@@ -4644,7 +4633,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="120" hidden="1">
+    <row r="4" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>156</v>
       </c>
@@ -4670,7 +4659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="140.1" hidden="1">
+    <row r="5" spans="1:8" ht="140" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>159</v>
       </c>
@@ -4696,7 +4685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="6" spans="1:8" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>162</v>
       </c>
@@ -4719,7 +4708,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="219.95" hidden="1">
+    <row r="7" spans="1:8" ht="220" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>164</v>
       </c>
@@ -4745,7 +4734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="8" spans="1:8" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>166</v>
       </c>
@@ -4768,7 +4757,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="120" hidden="1">
+    <row r="9" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>168</v>
       </c>
@@ -4791,7 +4780,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="10" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>170</v>
       </c>
@@ -4817,7 +4806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="103.35" hidden="1" customHeight="1">
+    <row r="11" spans="1:8" ht="103.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>172</v>
       </c>
@@ -4843,7 +4832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="100.35" hidden="1" customHeight="1">
+    <row r="12" spans="1:8" ht="100.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>174</v>
       </c>
@@ -4867,7 +4856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="13" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4888,7 +4877,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="80.099999999999994" hidden="1">
+    <row r="14" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>176</v>
       </c>
@@ -4909,7 +4898,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="80.099999999999994" hidden="1">
+    <row r="15" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>177</v>
       </c>
@@ -4928,7 +4917,7 @@
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" hidden="1">
+    <row r="16" spans="1:8" ht="20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>178</v>
       </c>
@@ -4949,7 +4938,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="17" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>179</v>
       </c>
@@ -4970,7 +4959,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.100000000000001" hidden="1">
+    <row r="18" spans="1:8" ht="20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>180</v>
       </c>
@@ -4991,7 +4980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="19" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>181</v>
       </c>
@@ -5012,7 +5001,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="76.349999999999994" hidden="1" customHeight="1">
+    <row r="20" spans="1:8" ht="76.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>182</v>
       </c>
@@ -5036,7 +5025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="76.349999999999994" hidden="1" customHeight="1">
+    <row r="21" spans="1:8" ht="76.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>183</v>
       </c>
@@ -5060,7 +5049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="60" hidden="1">
+    <row r="22" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>184</v>
       </c>
@@ -5081,7 +5070,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="23" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>185</v>
       </c>
@@ -5102,7 +5091,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="24" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>186</v>
       </c>
@@ -5123,7 +5112,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="25" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>187</v>
       </c>
@@ -5144,7 +5133,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="60" hidden="1">
+    <row r="26" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -5165,7 +5154,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60" hidden="1">
+    <row r="27" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>189</v>
       </c>
@@ -5186,7 +5175,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60" hidden="1">
+    <row r="28" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>190</v>
       </c>
@@ -5207,7 +5196,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60" hidden="1">
+    <row r="29" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>191</v>
       </c>
@@ -5228,7 +5217,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="99.95" hidden="1">
+    <row r="30" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>192</v>
       </c>
@@ -5249,7 +5238,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="60" hidden="1">
+    <row r="31" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>193</v>
       </c>
@@ -5270,7 +5259,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="60" hidden="1">
+    <row r="32" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>194</v>
       </c>
@@ -5291,7 +5280,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="33" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>195</v>
       </c>
@@ -5312,7 +5301,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="60" hidden="1">
+    <row r="34" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>196</v>
       </c>
@@ -5333,7 +5322,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="35" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>197</v>
       </c>
@@ -5354,7 +5343,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="36" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>198</v>
       </c>
@@ -5375,7 +5364,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="60" hidden="1">
+    <row r="37" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>199</v>
       </c>
@@ -5396,7 +5385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="279.95" hidden="1">
+    <row r="38" spans="1:8" ht="280" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>200</v>
       </c>
@@ -5422,7 +5411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="39" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>201</v>
       </c>
@@ -5443,7 +5432,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -5451,7 +5440,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8" ht="120.75" hidden="1" customHeight="1">
+    <row r="41" spans="1:8" ht="120.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>202</v>
       </c>
@@ -5477,7 +5466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="120" hidden="1">
+    <row r="42" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>203</v>
       </c>
@@ -5503,7 +5492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="140.1" hidden="1">
+    <row r="43" spans="1:8" ht="140" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>204</v>
       </c>
@@ -5529,7 +5518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="44" spans="1:8" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>205</v>
       </c>
@@ -5555,7 +5544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="219.95" hidden="1">
+    <row r="45" spans="1:8" ht="220" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>206</v>
       </c>
@@ -5581,7 +5570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="39.950000000000003" hidden="1">
+    <row r="46" spans="1:8" ht="40" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>207</v>
       </c>
@@ -5599,7 +5588,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="60" hidden="1">
+    <row r="47" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>208</v>
       </c>
@@ -5617,7 +5606,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="48" spans="1:8" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>209</v>
       </c>
@@ -5643,7 +5632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="120" hidden="1">
+    <row r="49" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>210</v>
       </c>
@@ -5669,7 +5658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="50" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>211</v>
       </c>
@@ -5695,7 +5684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="16"/>
       <c r="B51" s="19"/>
       <c r="C51" s="17"/>
@@ -5705,7 +5694,7 @@
       <c r="G51" s="28"/>
       <c r="H51" s="18"/>
     </row>
-    <row r="52" spans="1:8" ht="80.099999999999994" hidden="1">
+    <row r="52" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="s">
         <v>212</v>
       </c>
@@ -5731,7 +5720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="99.95" hidden="1">
+    <row r="53" spans="1:8" ht="100" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
         <v>214</v>
       </c>
@@ -5757,7 +5746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="159.94999999999999" hidden="1">
+    <row r="54" spans="1:8" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
         <v>216</v>
       </c>
@@ -5783,7 +5772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="120" hidden="1">
+    <row r="55" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>218</v>
       </c>
@@ -5809,7 +5798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="198.6" hidden="1" customHeight="1">
+    <row r="56" spans="1:8" ht="198.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
         <v>220</v>
       </c>
@@ -5835,7 +5824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="171.6" hidden="1" customHeight="1">
+    <row r="57" spans="1:8" ht="171.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>222</v>
       </c>
@@ -5861,7 +5850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="180" hidden="1">
+    <row r="58" spans="1:8" ht="180" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="16" t="s">
         <v>224</v>
       </c>
@@ -5887,7 +5876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="227.45" hidden="1" customHeight="1">
+    <row r="59" spans="1:8" ht="227.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>226</v>
       </c>
@@ -5913,7 +5902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="138" hidden="1" customHeight="1">
+    <row r="60" spans="1:8" ht="138" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="s">
         <v>228</v>
       </c>
@@ -5939,7 +5928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="320.10000000000002" hidden="1">
+    <row r="61" spans="1:8" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>230</v>
       </c>
@@ -5965,7 +5954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="221.1" hidden="1" customHeight="1">
+    <row r="62" spans="1:8" ht="221" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="16" t="s">
         <v>232</v>
       </c>
@@ -5991,7 +5980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -6001,7 +5990,7 @@
       <c r="G63" s="20"/>
       <c r="H63" s="18"/>
     </row>
-    <row r="64" spans="1:8" ht="264.75">
+    <row r="64" spans="1:8" ht="280" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="s">
         <v>234</v>
       </c>
@@ -6028,7 +6017,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="170.25">
+    <row r="65" spans="1:8" ht="140" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>236</v>
       </c>
@@ -6055,7 +6044,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="113.25">
+    <row r="66" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
         <v>238</v>
       </c>
@@ -6082,7 +6071,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="170.25">
+    <row r="67" spans="1:8" ht="140" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>240</v>
       </c>
@@ -6109,7 +6098,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="189">
+    <row r="68" spans="1:8" ht="180" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>242</v>
       </c>
@@ -6136,7 +6125,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="132">
+    <row r="69" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>244</v>
       </c>
@@ -6160,10 +6149,10 @@
         <v>46003</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="264.75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>246</v>
       </c>
@@ -6190,12 +6179,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="264.75">
+    <row r="71" spans="1:8" ht="240" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>248</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>249</v>
       </c>
       <c r="C71" s="17">
         <f>ROW() - ROW(TablaBacklog[[#Headers],[ID]]) - 2</f>
@@ -6214,15 +6203,15 @@
         <v>46003</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="264.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="260" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>250</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>251</v>
       </c>
       <c r="C72" s="12">
         <f>ROW() - ROW(TablaBacklog[[#Headers],[ID]]) - 2</f>
@@ -6241,15 +6230,15 @@
         <v>46003</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="132">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="140" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B73" s="17" t="s">
         <v>252</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>253</v>
       </c>
       <c r="C73" s="17">
         <f>ROW() - ROW(TablaBacklog[[#Headers],[ID]]) - 2</f>
@@ -6271,9 +6260,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="94.5">
+    <row r="74" spans="1:8" ht="100" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B74" s="12"/>
       <c r="C74" s="12">
@@ -6293,12 +6282,12 @@
         <v>46003</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="37.5">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="40" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B75" s="17"/>
       <c r="C75" s="17">
@@ -6321,12 +6310,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="75.75">
+    <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" s="17" t="s">
         <v>256</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>257</v>
       </c>
       <c r="C76" s="1">
         <f>ROW() - ROW(TablaBacklog[[#Headers],[ID]]) - 2</f>
@@ -6348,9 +6337,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="57">
+    <row r="77" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B77" s="17"/>
       <c r="C77" s="1">
@@ -6374,71 +6363,70 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"I"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D77">
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="Baja"/>
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="Media"/>
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="Alta"/>
+    <cfRule type="containsText" dxfId="17" priority="26" operator="containsText" text="Baja"/>
+    <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="Media"/>
+    <cfRule type="containsText" dxfId="15" priority="28" operator="containsText" text="Alta"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Bajo"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Medio"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"Alto"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F77">
-    <cfRule type="containsText" dxfId="24" priority="19" operator="containsText" text="Completo"/>
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="En progreso"/>
-    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Bloqueado"/>
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="Pendiente"/>
+    <cfRule type="containsText" dxfId="11" priority="19" operator="containsText" text="Completo"/>
+    <cfRule type="containsText" dxfId="10" priority="20" operator="containsText" text="En progreso"/>
+    <cfRule type="containsText" dxfId="9" priority="21" operator="containsText" text="Bloqueado"/>
+    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="Pendiente"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H42">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
-      <formula>"En progreso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H77">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"En progreso"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H77">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
-      <formula>"En progreso"</formula>
+  <conditionalFormatting sqref="H44:H45 H76:H1048576">
+    <cfRule type="cellIs" dxfId="2" priority="17" operator="equal">
+      <formula>"Pendiente"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
+      <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44:H45 H76:H1048576">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+  <conditionalFormatting sqref="H76:H1048576">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
       <formula>"En progreso"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
-      <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">

</xml_diff>

<commit_message>
Todo listo para la demo
</commit_message>
<xml_diff>
--- a/Planificación_ISO.xlsx
+++ b/Planificación_ISO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceu365-my.sharepoint.com/personal/victor_vegamartinez_usp_ceu_es/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfre\workspace\cuartoDeCarrera\ISO\Proyecto_Ingenieria_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD454BBD-C0DE-4390-A0E6-49C59043E0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C81DEEF-562C-4A68-A8F7-77BF3D406026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -952,7 +952,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1235,204 +1235,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="60">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF95B3D7"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1851,6 +1653,204 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF95B3D7"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1865,23 +1865,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TablaBacklog" displayName="TablaBacklog" ref="A1:H77" headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TablaBacklog" displayName="TablaBacklog" ref="A1:H77" headerRowDxfId="59" dataDxfId="58" totalsRowDxfId="57">
   <autoFilter ref="A1:H77" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
     <filterColumn colId="6">
-      <filters blank="1">
+      <filters>
         <dateGroupItem year="2025" month="12" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{702BA59E-E87C-AF43-BC72-116919A29E64}" name="Criterio de validacion" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6924BD28-A9A8-B84F-AE98-42459B25AAE0}" name="ID" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priority" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tiempo planning poker (horas)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Entrega" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{2C9703D9-E678-1342-81C4-A1629A8FA8A2}" name="Estado" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{702BA59E-E87C-AF43-BC72-116919A29E64}" name="Criterio de validacion" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{6924BD28-A9A8-B84F-AE98-42459B25AAE0}" name="ID" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Priority" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tiempo planning poker (horas)" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Entrega" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{2C9703D9-E678-1342-81C4-A1629A8FA8A2}" name="Estado" dataDxfId="49" totalsRowDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2174,21 +2174,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E8B59A-7A92-E349-A281-22786FC7C0A0}">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A104" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" style="10" customWidth="1"/>
     <col min="4" max="4" width="36" style="10" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="36">
+    <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36">
+    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36">
+    <row r="7" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36">
+    <row r="11" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="54">
+    <row r="13" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="36">
+    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="36">
+    <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="36">
+    <row r="16" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36">
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="36">
+    <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="36">
+    <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="36">
+    <row r="21" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="36">
+    <row r="22" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18">
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18">
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="36">
+    <row r="25" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="36">
+    <row r="27" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="36">
+    <row r="28" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18">
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="36">
+    <row r="30" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="36">
+    <row r="31" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="54">
+    <row r="32" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>45</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="36">
+    <row r="33" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="36">
+    <row r="34" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="36">
+    <row r="35" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="36">
+    <row r="36" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>49</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="36">
+    <row r="37" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>53</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36">
+    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="36">
+    <row r="41" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="36">
+    <row r="42" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18">
+    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>56</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18">
+    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="54">
+    <row r="45" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="54">
+    <row r="46" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>59</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="36">
+    <row r="47" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>60</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="36">
+    <row r="48" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>61</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18">
+    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>62</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="36">
+    <row r="50" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>63</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="54">
+    <row r="51" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>64</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="36">
+    <row r="52" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>65</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="36">
+    <row r="53" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="54">
+    <row r="54" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>67</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="54">
+    <row r="55" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>68</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="54">
+    <row r="56" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>69</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="36">
+    <row r="57" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="54">
+    <row r="58" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>71</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="54">
+    <row r="59" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>72</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="36">
+    <row r="60" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="54">
+    <row r="61" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>75</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="36">
+    <row r="62" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>76</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="36">
+    <row r="63" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>77</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="36">
+    <row r="64" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>78</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="36">
+    <row r="65" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>79</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="36">
+    <row r="66" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>80</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="54">
+    <row r="67" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>81</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="36">
+    <row r="68" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>84</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="54">
+    <row r="69" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>85</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="36">
+    <row r="70" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>87</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="36">
+    <row r="71" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>88</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="36">
+    <row r="72" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>90</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="36">
+    <row r="73" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>91</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="18">
+    <row r="74" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>94</v>
       </c>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="18">
+    <row r="75" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>95</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="36">
+    <row r="76" spans="1:15" ht="36" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>96</v>
       </c>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="M76" s="38"/>
     </row>
-    <row r="77" spans="1:15" ht="36">
+    <row r="77" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>97</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="54">
+    <row r="78" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>98</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="54">
+    <row r="79" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>99</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="36">
+    <row r="80" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>100</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="18">
+    <row r="81" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>39</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="36">
+    <row r="82" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>101</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="54">
+    <row r="83" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>102</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="54">
+    <row r="84" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>103</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="36">
+    <row r="85" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>104</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="18">
+    <row r="86" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>105</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="18">
+    <row r="87" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>106</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="18">
+    <row r="88" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>107</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="36">
+    <row r="89" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>108</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="36">
+    <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>109</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="36">
+    <row r="91" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>110</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="18">
+    <row r="92" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>111</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="18">
+    <row r="93" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>112</v>
       </c>
@@ -4072,13 +4072,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="18">
+    <row r="94" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D94" s="32"/>
     </row>
-    <row r="95" spans="1:6" ht="18">
+    <row r="95" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>114</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="54">
+    <row r="96" spans="1:6" ht="54" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>115</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="35" customFormat="1" ht="55.9" customHeight="1">
+    <row r="97" spans="1:6" s="35" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>117</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="35" customFormat="1" ht="72">
+    <row r="98" spans="1:6" s="35" customFormat="1" ht="72" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>119</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="99" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>120</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="35" customFormat="1" ht="55.15" customHeight="1">
+    <row r="100" spans="1:6" s="35" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>121</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="35" customFormat="1" ht="54">
+    <row r="101" spans="1:6" s="35" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>122</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="102" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>124</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="35" customFormat="1" ht="78.400000000000006" customHeight="1">
+    <row r="103" spans="1:6" s="35" customFormat="1" ht="78.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>125</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="104" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>127</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="105" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>128</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" s="35" customFormat="1" ht="54">
+    <row r="106" spans="1:6" s="35" customFormat="1" ht="54" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>129</v>
       </c>
@@ -4310,7 +4310,7 @@
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
     </row>
-    <row r="107" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="107" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>130</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="35" customFormat="1" ht="18">
+    <row r="108" spans="1:6" s="35" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A108" s="4"/>
       <c r="B108" s="36">
         <f>+Requisitos!C59</f>
@@ -4350,7 +4350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="109" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>131</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="110" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A110" s="37" t="s">
         <v>132</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="35" customFormat="1" ht="18">
+    <row r="111" spans="1:6" s="35" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>133</v>
       </c>
@@ -4402,7 +4402,7 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
     </row>
-    <row r="112" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="112" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A112" s="37" t="s">
         <v>134</v>
       </c>
@@ -4412,7 +4412,7 @@
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
     </row>
-    <row r="113" spans="1:6" s="35" customFormat="1" ht="18">
+    <row r="113" spans="1:6" s="35" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A113" s="3"/>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
@@ -4420,7 +4420,7 @@
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
     </row>
-    <row r="114" spans="1:6" s="35" customFormat="1" ht="36">
+    <row r="114" spans="1:6" s="35" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>135</v>
       </c>
@@ -4430,7 +4430,7 @@
       <c r="E114" s="34"/>
       <c r="F114" s="34"/>
     </row>
-    <row r="115" spans="1:6" ht="18">
+    <row r="115" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>136</v>
       </c>
@@ -4440,7 +4440,7 @@
       <c r="E115" s="34"/>
       <c r="F115" s="34"/>
     </row>
-    <row r="116" spans="1:6" ht="18">
+    <row r="116" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A116" s="35" t="s">
         <v>137</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="18">
+    <row r="117" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A117" s="35">
         <v>64.650000000000006</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>66.709999999999994</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>139</v>
       </c>
@@ -4475,53 +4475,53 @@
   </sheetData>
   <autoFilter ref="A1:F32" xr:uid="{74E8B59A-7A92-E349-A281-22786FC7C0A0}"/>
   <conditionalFormatting sqref="B107">
-    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109:C109">
-    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="55" priority="8" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="54" priority="9" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="43" priority="8" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="42" priority="9" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C86 B46:B47 B87 C88:D88 C89:C93">
-    <cfRule type="containsText" dxfId="53" priority="25" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="52" priority="26" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="51" priority="27" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="39" priority="27" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:C97">
-    <cfRule type="containsText" dxfId="50" priority="22" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="49" priority="23" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="48" priority="24" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="38" priority="22" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="37" priority="23" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="36" priority="24" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99:C101">
-    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="35" priority="19" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="34" priority="20" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="33" priority="21" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103">
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="43" priority="14" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105:C107">
-    <cfRule type="containsText" dxfId="41" priority="10" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="40" priority="11" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="39" priority="12" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="27" priority="12" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111:C113">
-    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="Bajo"/>
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="Medio"/>
-    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="Alto"/>
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="Bajo"/>
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="Medio"/>
+    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="Alto"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
       <formula>"En progreso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4542,24 +4542,24 @@
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58" style="1" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="70.900000000000006" customHeight="1">
+    <row r="1" spans="1:8" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>140</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="270" hidden="1">
+    <row r="2" spans="1:8" ht="270" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>147</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="126">
+    <row r="3" spans="1:8" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="108" hidden="1">
+    <row r="4" spans="1:8" ht="108" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>156</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="126" hidden="1">
+    <row r="5" spans="1:8" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>159</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="144">
+    <row r="6" spans="1:8" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>162</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="216" hidden="1">
+    <row r="7" spans="1:8" ht="216" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>164</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="162">
+    <row r="8" spans="1:8" ht="162" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>166</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="126">
+    <row r="9" spans="1:8" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>168</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="198" hidden="1">
+    <row r="10" spans="1:8" ht="198" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>170</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="103.15" hidden="1" customHeight="1">
+    <row r="11" spans="1:8" ht="103.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>172</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="100.15" hidden="1" customHeight="1">
+    <row r="12" spans="1:8" ht="100.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>174</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="54">
+    <row r="13" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>175</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="72">
+    <row r="14" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>176</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="90">
+    <row r="15" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>177</v>
       </c>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="36">
+    <row r="16" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>178</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="36">
+    <row r="17" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>179</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="36">
+    <row r="18" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>180</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="36">
+    <row r="19" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>181</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="76.150000000000006" hidden="1" customHeight="1">
+    <row r="20" spans="1:8" ht="76.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>182</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="76.150000000000006" hidden="1" customHeight="1">
+    <row r="21" spans="1:8" ht="76.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>183</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="54">
+    <row r="22" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>184</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="54">
+    <row r="23" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>185</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="36">
+    <row r="24" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>186</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="36">
+    <row r="25" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>187</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="54">
+    <row r="26" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="54">
+    <row r="27" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>189</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="72">
+    <row r="28" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>190</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="54">
+    <row r="29" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>191</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="108">
+    <row r="30" spans="1:8" ht="108" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>192</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="54">
+    <row r="31" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>193</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="54">
+    <row r="32" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>194</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="36">
+    <row r="33" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>195</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="72">
+    <row r="34" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>196</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="54">
+    <row r="35" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>197</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="36">
+    <row r="36" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>198</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="54">
+    <row r="37" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>199</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="270" hidden="1">
+    <row r="38" spans="1:8" ht="270" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>200</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="54">
+    <row r="39" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>201</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -5441,7 +5441,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8" ht="120.75" hidden="1" customHeight="1">
+    <row r="41" spans="1:8" ht="120.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>202</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="108" hidden="1">
+    <row r="42" spans="1:8" ht="108" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>203</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="126" hidden="1">
+    <row r="43" spans="1:8" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>204</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="144" hidden="1">
+    <row r="44" spans="1:8" ht="144" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21" t="s">
         <v>205</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="216" hidden="1">
+    <row r="45" spans="1:8" ht="216" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25" t="s">
         <v>206</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="36">
+    <row r="46" spans="1:8" ht="36" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>207</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="54">
+    <row r="47" spans="1:8" ht="54" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
         <v>208</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="162" hidden="1">
+    <row r="48" spans="1:8" ht="162" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>209</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="126" hidden="1">
+    <row r="49" spans="1:8" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
         <v>210</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="198" hidden="1">
+    <row r="50" spans="1:8" ht="198" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>211</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16"/>
       <c r="B51" s="19"/>
       <c r="C51" s="17"/>
@@ -5695,7 +5695,7 @@
       <c r="G51" s="28"/>
       <c r="H51" s="18"/>
     </row>
-    <row r="52" spans="1:8" ht="72" hidden="1">
+    <row r="52" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
         <v>212</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="126" hidden="1">
+    <row r="53" spans="1:8" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
         <v>214</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="162" hidden="1">
+    <row r="54" spans="1:8" ht="162" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
         <v>216</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="108" hidden="1">
+    <row r="55" spans="1:8" ht="108" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>218</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="198.4" hidden="1" customHeight="1">
+    <row r="56" spans="1:8" ht="198.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
         <v>220</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="171.4" hidden="1" customHeight="1">
+    <row r="57" spans="1:8" ht="171.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>222</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="162" hidden="1">
+    <row r="58" spans="1:8" ht="162" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
         <v>224</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="227.65" hidden="1" customHeight="1">
+    <row r="59" spans="1:8" ht="227.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>226</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="138" hidden="1" customHeight="1">
+    <row r="60" spans="1:8" ht="138" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
         <v>228</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="288" hidden="1">
+    <row r="61" spans="1:8" ht="288" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>230</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="220.9" hidden="1" customHeight="1">
+    <row r="62" spans="1:8" ht="220.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
         <v>232</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -5991,7 +5991,7 @@
       <c r="G63" s="20"/>
       <c r="H63" s="18"/>
     </row>
-    <row r="64" spans="1:8" ht="302.25">
+    <row r="64" spans="1:8" ht="288" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
         <v>234</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="151.5">
+    <row r="65" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>236</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="151.5">
+    <row r="66" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A66" s="16" t="s">
         <v>238</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="144">
+    <row r="67" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>240</v>
       </c>
@@ -6096,10 +6096,10 @@
         <v>46003</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="162">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="162" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>242</v>
       </c>
@@ -6123,10 +6123,10 @@
         <v>46003</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>244</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="252">
+    <row r="70" spans="1:8" ht="252" x14ac:dyDescent="0.3">
       <c r="A70" s="16" t="s">
         <v>246</v>
       </c>
@@ -6177,10 +6177,10 @@
         <v>46003</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="252">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="252" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
         <v>248</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="252">
+    <row r="72" spans="1:8" ht="252" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>250</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="132">
+    <row r="73" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A73" s="16" t="s">
         <v>252</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="90">
+    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>254</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="36">
+    <row r="75" spans="1:8" ht="36" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
         <v>255</v>
       </c>
@@ -6308,10 +6308,10 @@
         <v>46003</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="54" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>256</v>
       </c>
@@ -6335,10 +6335,10 @@
         <v>46003</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="54" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>258</v>
       </c>
@@ -6359,74 +6359,74 @@
         <v>46003</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="32" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"I"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D77">
-    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="Baja"/>
-    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="Media"/>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Alta"/>
+    <cfRule type="containsText" dxfId="17" priority="26" operator="containsText" text="Baja"/>
+    <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="Media"/>
+    <cfRule type="containsText" dxfId="15" priority="28" operator="containsText" text="Alta"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Bajo"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"Medio"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"Alto"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F77">
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="Completo"/>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="En progreso"/>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Bloqueado"/>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Pendiente"/>
+    <cfRule type="containsText" dxfId="11" priority="19" operator="containsText" text="Completo"/>
+    <cfRule type="containsText" dxfId="10" priority="20" operator="containsText" text="En progreso"/>
+    <cfRule type="containsText" dxfId="9" priority="21" operator="containsText" text="Bloqueado"/>
+    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="Pendiente"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H42">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H77">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"En progreso"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:H45 H76:H1048576">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="17" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
       <formula>"Completado"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76:H1048576">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
       <formula>"En progreso"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6451,4 +6451,284 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009DF1A11783FCDC41A7A321B5C8820943" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ce22d73d212400d0dce74983523ad93d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3095d5c1-7116-4670-aa9b-a30d907ab454" xmlns:ns4="b0916ef2-55b0-459d-a239-3af1ebdd1540" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89cb6bf1a9b146548b183cc26538a8b3" ns3:_="" ns4:_="">
+    <xsd:import namespace="3095d5c1-7116-4670-aa9b-a30d907ab454"/>
+    <xsd:import namespace="b0916ef2-55b0-459d-a239-3af1ebdd1540"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3095d5c1-7116-4670-aa9b-a30d907ab454" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="13" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="15" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="16" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="20" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b0916ef2-55b0-459d-a239-3af1ebdd1540" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Hash de la sugerencia para compartir" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3095d5c1-7116-4670-aa9b-a30d907ab454" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E520DA28-119D-4B08-9127-3379D5CF8118}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F19DE960-4053-4B19-A5F1-8D5EB28BDE48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3095d5c1-7116-4670-aa9b-a30d907ab454"/>
+    <ds:schemaRef ds:uri="b0916ef2-55b0-459d-a239-3af1ebdd1540"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D0F4C61-7A29-480B-B405-A9B89ADA3718}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b0916ef2-55b0-459d-a239-3af1ebdd1540"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3095d5c1-7116-4670-aa9b-a30d907ab454"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>